<commit_message>
related symptoms generator added
</commit_message>
<xml_diff>
--- a/app/src/db_population/Conditions_and_symptoms.xlsx
+++ b/app/src/db_population/Conditions_and_symptoms.xlsx
@@ -4,12 +4,12 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25660" windowHeight="14560" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15440" windowHeight="13580" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="140000" concurrentCalc="0"/>
+  <calcPr calcId="140000" iterateDelta="1E-4" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="57">
   <si>
     <t>name</t>
   </si>
@@ -36,9 +36,6 @@
     <t>hangover</t>
   </si>
   <si>
-    <t>malaise, dehydration, dizziness, fatigue, lightheadedness, loss of appetite, thirst, vertigo, sweating, diarrhea, heartburn, indigestion, nausea, vomiting, sensitivity to light, sensitivity to sound,headache, excess urination, fast heart rate, irritability, sleepiness</t>
-  </si>
-  <si>
     <t>Unpleasant symptoms that occur after excessive alcohol intake.</t>
   </si>
   <si>
@@ -72,9 +69,6 @@
     <t>Congrats! You're having a baby</t>
   </si>
   <si>
-    <t>dry cough, cough with phlegm, chronic cough,  fatigue, malaise, runny nose, post-nasal drip, chest pressure, headache, shortness of breath, sleeping difficulty, sore throat</t>
-  </si>
-  <si>
     <t>cough, cough with phlegm, congestion, runny nose, sneezing, loss of smell, redness, post-nasal drip, chills, fatigue, fever, malaise, body ache, watery eyes, eye itchiness, eye redness, sinus pressure, chest pressure, headache, sore throat, throat irritation</t>
   </si>
   <si>
@@ -102,9 +96,6 @@
     <t>Testicular torsion</t>
   </si>
   <si>
-    <t>testicular pain, abdominal pain, nausea, vomiting, scrotal selling, scrotal tenderness</t>
-  </si>
-  <si>
     <t>testicular torsion</t>
   </si>
   <si>
@@ -178,16 +169,60 @@
   </si>
   <si>
     <t>cond_12</t>
+  </si>
+  <si>
+    <t>malaise, dehydration, dizziness, fatigue, lightheadedness, loss of appetite, thirst, vertigo, sweating, diarrhea, heartburn, indigestion, nausea, vomiting, sensitivity to light, sensitivity to sound, headache, excess urination, fast heart rate, irritability, sleepiness</t>
+  </si>
+  <si>
+    <t>testicular pain, abdominal pain, nausea, vomiting, scrotal swelling, scrotal tenderness</t>
+  </si>
+  <si>
+    <t>dry cough, cough with phlegm, chronic cough, fatigue, malaise, runny nose, post-nasal drip, chest pressure, headache, shortness of breath, difficulty sleeping, sore throat</t>
+  </si>
+  <si>
+    <t>age_min</t>
+  </si>
+  <si>
+    <t>age_max</t>
+  </si>
+  <si>
+    <t>time_min</t>
+  </si>
+  <si>
+    <t>time_max</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -210,14 +245,19 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -547,17 +587,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E13"/>
+  <dimension ref="A1:I13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="2" max="2" width="18.83203125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:9">
       <c r="A1" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -569,211 +612,367 @@
         <v>2</v>
       </c>
       <c r="E1" t="s">
+        <v>53</v>
+      </c>
+      <c r="F1" t="s">
+        <v>54</v>
+      </c>
+      <c r="G1" t="s">
+        <v>55</v>
+      </c>
+      <c r="H1" t="s">
+        <v>56</v>
+      </c>
+      <c r="I1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:9">
       <c r="A2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <v>6</v>
+      </c>
+      <c r="F2">
+        <v>40</v>
+      </c>
+      <c r="G2">
+        <v>2</v>
+      </c>
+      <c r="H2">
+        <v>3</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
+      <c r="A3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <v>6</v>
+      </c>
+      <c r="F3">
+        <v>100</v>
+      </c>
+      <c r="G3">
+        <v>10</v>
+      </c>
+      <c r="H3">
+        <v>14</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
+      <c r="A4" t="s">
+        <v>40</v>
+      </c>
+      <c r="B4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
+      <c r="F4">
+        <v>100</v>
+      </c>
+      <c r="G4">
+        <v>7</v>
+      </c>
+      <c r="H4">
+        <v>10</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
+      <c r="A5" t="s">
         <v>41</v>
       </c>
-      <c r="B2" t="s">
-        <v>29</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="D2">
-        <v>0</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5">
-      <c r="A3" t="s">
+      <c r="B5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5">
+        <v>3</v>
+      </c>
+      <c r="F5">
+        <v>100</v>
+      </c>
+      <c r="G5">
+        <v>5</v>
+      </c>
+      <c r="H5">
+        <v>10</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9">
+      <c r="A6" t="s">
         <v>42</v>
-      </c>
-      <c r="B3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D3">
-        <v>0</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5">
-      <c r="A4" t="s">
-        <v>43</v>
-      </c>
-      <c r="B4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D4">
-        <v>0</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5">
-      <c r="A5" t="s">
-        <v>44</v>
-      </c>
-      <c r="B5" t="s">
-        <v>9</v>
-      </c>
-      <c r="C5" t="s">
-        <v>10</v>
-      </c>
-      <c r="D5">
-        <v>0</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5">
-      <c r="A6" t="s">
-        <v>45</v>
       </c>
       <c r="B6" t="s">
         <v>4</v>
       </c>
       <c r="C6" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="E6" s="2">
+        <v>18</v>
+      </c>
+      <c r="F6" s="2">
+        <v>100</v>
+      </c>
+      <c r="G6" s="2">
+        <v>1</v>
+      </c>
+      <c r="H6" s="2">
+        <v>2</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9">
+      <c r="A7" t="s">
+        <v>43</v>
+      </c>
+      <c r="B7" t="s">
+        <v>23</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="E7" s="2">
+        <v>41</v>
+      </c>
+      <c r="F7" s="2">
+        <v>100</v>
+      </c>
+      <c r="G7" s="2">
+        <v>5</v>
+      </c>
+      <c r="H7" s="2">
+        <v>21</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9">
+      <c r="A8" t="s">
+        <v>44</v>
+      </c>
+      <c r="B8" t="s">
+        <v>29</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+      <c r="E8">
+        <v>0</v>
+      </c>
+      <c r="F8">
+        <v>100</v>
+      </c>
+      <c r="G8">
+        <v>0.1</v>
+      </c>
+      <c r="H8">
+        <v>1</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9">
+      <c r="A9" t="s">
+        <v>45</v>
+      </c>
+      <c r="B9" t="s">
         <v>6</v>
       </c>
-      <c r="D6">
-        <v>0</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5">
-      <c r="A7" t="s">
-        <v>46</v>
-      </c>
-      <c r="B7" t="s">
-        <v>25</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="D7">
-        <v>0</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5">
-      <c r="A8" t="s">
-        <v>47</v>
-      </c>
-      <c r="B8" t="s">
-        <v>32</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="D8">
-        <v>0</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5">
-      <c r="A9" t="s">
-        <v>48</v>
-      </c>
-      <c r="B9" t="s">
-        <v>7</v>
-      </c>
       <c r="C9" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D9">
         <v>1</v>
       </c>
-      <c r="E9" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5">
+      <c r="E9">
+        <v>13</v>
+      </c>
+      <c r="F9">
+        <v>45</v>
+      </c>
+      <c r="G9">
+        <v>30</v>
+      </c>
+      <c r="H9">
+        <v>270</v>
+      </c>
+      <c r="I9" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9">
       <c r="A10" t="s">
+        <v>46</v>
+      </c>
+      <c r="B10" t="s">
+        <v>34</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+      <c r="E10">
+        <v>0</v>
+      </c>
+      <c r="F10">
+        <v>100</v>
+      </c>
+      <c r="G10">
+        <v>2</v>
+      </c>
+      <c r="H10">
+        <v>10</v>
+      </c>
+      <c r="I10" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9">
+      <c r="A11" t="s">
+        <v>47</v>
+      </c>
+      <c r="B11" t="s">
+        <v>20</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D11">
+        <v>0</v>
+      </c>
+      <c r="E11">
+        <v>19</v>
+      </c>
+      <c r="F11">
+        <v>100</v>
+      </c>
+      <c r="G11">
+        <v>14</v>
+      </c>
+      <c r="H11">
+        <v>30</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9">
+      <c r="A12" t="s">
+        <v>48</v>
+      </c>
+      <c r="B12" t="s">
+        <v>17</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D12">
+        <v>0</v>
+      </c>
+      <c r="E12">
+        <v>6</v>
+      </c>
+      <c r="F12">
+        <v>18</v>
+      </c>
+      <c r="G12">
+        <v>1</v>
+      </c>
+      <c r="H12">
+        <v>5</v>
+      </c>
+      <c r="I12" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9">
+      <c r="A13" t="s">
         <v>49</v>
       </c>
-      <c r="B10" t="s">
-        <v>37</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="D10">
-        <v>0</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5">
-      <c r="A11" t="s">
-        <v>50</v>
-      </c>
-      <c r="B11" t="s">
-        <v>22</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="D11">
-        <v>0</v>
-      </c>
-      <c r="E11" s="1" t="s">
+      <c r="B13" t="s">
+        <v>25</v>
+      </c>
+      <c r="C13" s="1" t="s">
         <v>24</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5">
-      <c r="A12" t="s">
-        <v>51</v>
-      </c>
-      <c r="B12" t="s">
-        <v>19</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="D12">
-        <v>0</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5">
-      <c r="A13" t="s">
-        <v>52</v>
-      </c>
-      <c r="B13" t="s">
-        <v>28</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>26</v>
       </c>
       <c r="D13">
         <v>2</v>
       </c>
-      <c r="E13" s="1" t="s">
-        <v>27</v>
+      <c r="E13">
+        <v>3</v>
+      </c>
+      <c r="F13">
+        <v>40</v>
+      </c>
+      <c r="G13">
+        <v>0</v>
+      </c>
+      <c r="H13">
+        <v>0.33</v>
+      </c>
+      <c r="I13" s="1" t="s">
+        <v>51</v>
       </c>
     </row>
   </sheetData>
@@ -781,6 +980,7 @@
     <sortCondition ref="B2:B13"/>
   </sortState>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>